<commit_message>
Busqueda aleatoria y clic en articulo. Funcional
</commit_message>
<xml_diff>
--- a/src/test/resources/data/inventario.xlsx
+++ b/src/test/resources/data/inventario.xlsx
@@ -28,7 +28,7 @@
     <t xml:space="preserve">cantidad</t>
   </si>
   <si>
-    <t xml:space="preserve">taladro</t>
+    <t xml:space="preserve">televisor</t>
   </si>
   <si>
     <t xml:space="preserve">5</t>
@@ -107,7 +107,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -117,10 +117,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -148,7 +144,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -174,43 +170,43 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3"/>
-      <c r="B3" s="4"/>
+      <c r="B3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3"/>
-      <c r="B4" s="4"/>
+      <c r="B4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3"/>
-      <c r="B5" s="4"/>
+      <c r="B5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3"/>
-      <c r="B6" s="4"/>
+      <c r="B6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3"/>
-      <c r="B7" s="4"/>
+      <c r="B7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3"/>
-      <c r="B8" s="4"/>
+      <c r="B8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3"/>
-      <c r="B9" s="4"/>
+      <c r="B9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3"/>
-      <c r="B10" s="4"/>
+      <c r="B10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3"/>
-      <c r="B11" s="4"/>
+      <c r="B11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3"/>
-      <c r="B12" s="4"/>
+      <c r="B12" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Punto de Control 2
</commit_message>
<xml_diff>
--- a/src/test/resources/data/inventario.xlsx
+++ b/src/test/resources/data/inventario.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t xml:space="preserve">producto</t>
   </si>
@@ -32,6 +32,27 @@
   </si>
   <si>
     <t xml:space="preserve">5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tecnologia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">carro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">guadañadora</t>
+  </si>
+  <si>
+    <t xml:space="preserve">taladro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4</t>
   </si>
 </sst>
 </file>
@@ -107,7 +128,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -117,10 +138,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -144,7 +161,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -169,44 +186,60 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
producto en Excel Televisor + 10
</commit_message>
<xml_diff>
--- a/src/test/resources/data/inventario.xlsx
+++ b/src/test/resources/data/inventario.xlsx
@@ -28,10 +28,10 @@
     <t xml:space="preserve">cantidad</t>
   </si>
   <si>
-    <t xml:space="preserve">ropa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5</t>
+    <t xml:space="preserve">televisor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10</t>
   </si>
 </sst>
 </file>
@@ -140,7 +140,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>